<commit_message>
OAM Memory reads should return 0xFF while DMA is transfering data, more passing Mooneye test cases
</commit_message>
<xml_diff>
--- a/FrozenBoyTest/Status/TestStatus.xlsx
+++ b/FrozenBoyTest/Status/TestStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\frozen\Documents\03_programming\online\emulation\FrozenBoy\FrozenBoyTest\Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C31CA1-B820-4FF5-B9FE-11B1F377B44B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C7227C-56F6-415D-876C-B989979D4373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D8B7F7EE-952E-4020-9F78-05F1904D33E7}"/>
   </bookViews>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19764FC5-60A7-462C-BC39-C8650463AB7B}">
   <dimension ref="B2:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,7 +1044,7 @@
         <v>58</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.3">
@@ -1060,7 +1060,7 @@
         <v>60</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.3">
@@ -1156,7 +1156,7 @@
         <v>72</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.3">
@@ -1164,7 +1164,7 @@
         <v>73</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.3">
@@ -1172,7 +1172,7 @@
         <v>74</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.3">
@@ -1180,7 +1180,7 @@
         <v>75</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.3">
@@ -1188,7 +1188,7 @@
         <v>76</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.3">
@@ -1196,7 +1196,7 @@
         <v>77</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.3">
@@ -1228,7 +1228,7 @@
         <v>83</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="4:5" x14ac:dyDescent="0.3">
@@ -1236,7 +1236,7 @@
         <v>84</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="4:5" x14ac:dyDescent="0.3">
@@ -1252,7 +1252,7 @@
         <v>82</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="4:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
More games and some MBC1 tests
</commit_message>
<xml_diff>
--- a/FrozenBoyTest/Status/TestStatus.xlsx
+++ b/FrozenBoyTest/Status/TestStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\frozen\Documents\03_programming\online\emulation\FrozenBoy\FrozenBoyTest\Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC06F3C-546C-4E9E-83DF-D42C5E7C2CF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2337E2B6-C6AE-40C0-9D1C-A6488CB6A647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D8B7F7EE-952E-4020-9F78-05F1904D33E7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="101">
   <si>
     <t>Acceptance</t>
   </si>
@@ -292,6 +292,51 @@
   </si>
   <si>
     <t>rst_timing.gb</t>
+  </si>
+  <si>
+    <t>Emulator Only</t>
+  </si>
+  <si>
+    <t>bits_bank1.gb</t>
+  </si>
+  <si>
+    <t>bits_bank2.gb</t>
+  </si>
+  <si>
+    <t>bits_mode.gb</t>
+  </si>
+  <si>
+    <t>bits_ramg.gb</t>
+  </si>
+  <si>
+    <t>multicart_rom_8Mb.gb</t>
+  </si>
+  <si>
+    <t>ram_256kb.gb</t>
+  </si>
+  <si>
+    <t>ram_64kb.gb</t>
+  </si>
+  <si>
+    <t>rom_16Mb.gb</t>
+  </si>
+  <si>
+    <t>rom_1Mb.gb</t>
+  </si>
+  <si>
+    <t>rom_2Mb.gb</t>
+  </si>
+  <si>
+    <t>rom_4Mb.gb</t>
+  </si>
+  <si>
+    <t>rom_512kb.gb</t>
+  </si>
+  <si>
+    <t>rom_8Mb.gb</t>
+  </si>
+  <si>
+    <t>Runtime exception</t>
   </si>
 </sst>
 </file>
@@ -345,7 +390,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -689,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19764FC5-60A7-462C-BC39-C8650463AB7B}">
-  <dimension ref="B2:E77"/>
+  <dimension ref="B2:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,6 +767,7 @@
     <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
@@ -1159,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
         <v>73</v>
       </c>
@@ -1167,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
         <v>74</v>
       </c>
@@ -1175,7 +1242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
         <v>75</v>
       </c>
@@ -1183,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D68" t="s">
         <v>76</v>
       </c>
@@ -1191,7 +1258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D69" t="s">
         <v>77</v>
       </c>
@@ -1199,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D70" t="s">
         <v>78</v>
       </c>
@@ -1207,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D71" t="s">
         <v>79</v>
       </c>
@@ -1215,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D72" t="s">
         <v>80</v>
       </c>
@@ -1223,7 +1290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D73" t="s">
         <v>83</v>
       </c>
@@ -1231,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D74" t="s">
         <v>84</v>
       </c>
@@ -1239,7 +1306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D75" t="s">
         <v>81</v>
       </c>
@@ -1247,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D76" t="s">
         <v>82</v>
       </c>
@@ -1255,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D77" t="s">
         <v>85</v>
       </c>
@@ -1263,13 +1330,155 @@
         <v>2</v>
       </c>
     </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D80" t="s">
+        <v>88</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D81" t="s">
+        <v>89</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D82" t="s">
+        <v>90</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D83" t="s">
+        <v>91</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D84" t="s">
+        <v>92</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D85" t="s">
+        <v>93</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D86" t="s">
+        <v>94</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F86" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D87" t="s">
+        <v>95</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F87" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D88" t="s">
+        <v>96</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F88" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D89" t="s">
+        <v>97</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F89" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D90" t="s">
+        <v>98</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F90" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D91" t="s">
+        <v>99</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F91" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E1:E83 E85:E1048576">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Passed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MBC1 complete support and tests
</commit_message>
<xml_diff>
--- a/FrozenBoyTest/Status/TestStatus.xlsx
+++ b/FrozenBoyTest/Status/TestStatus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\frozen\Documents\03_programming\online\emulation\FrozenBoy\FrozenBoyTest\Status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2337E2B6-C6AE-40C0-9D1C-A6488CB6A647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6F6849-AC31-49D7-8CDC-A85DCE29C1AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D8B7F7EE-952E-4020-9F78-05F1904D33E7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="101">
   <si>
     <t>Acceptance</t>
   </si>
@@ -336,7 +336,7 @@
     <t>rom_8Mb.gb</t>
   </si>
   <si>
-    <t>Runtime exception</t>
+    <t>MBC1</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <font>
         <color theme="0"/>
@@ -411,6 +411,27 @@
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -755,10 +776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19764FC5-60A7-462C-BC39-C8650463AB7B}">
-  <dimension ref="B2:F91"/>
+  <dimension ref="B2:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1334,6 +1355,9 @@
       <c r="B79" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="C79" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D79" t="s">
         <v>87</v>
       </c>
@@ -1349,131 +1373,104 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D81" t="s">
         <v>89</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D82" t="s">
         <v>90</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D83" t="s">
         <v>91</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F83" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D84" t="s">
         <v>92</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D85" t="s">
         <v>93</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F85" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D86" t="s">
         <v>94</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F86" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D87" t="s">
         <v>95</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F87" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D88" t="s">
         <v>96</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F88" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D89" t="s">
         <v>97</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F89" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="90" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D90" t="s">
         <v>98</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F90" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="91" spans="4:6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D91" t="s">
         <v>99</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F91" t="s">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E83 E85:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="E86:E1048576 E1:E83">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E84:E91">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>

</xml_diff>